<commit_message>
Added a copy of Airflow dag
</commit_message>
<xml_diff>
--- a/StarSchemaPlan.xlsx
+++ b/StarSchemaPlan.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\IBA Course Material\CSE 609 - Data Analytics and Warehousing\Semester Project\dawh-project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03437852-A5FA-45F9-A28A-475AEE0B3833}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{520F888D-C5EB-48F7-81E0-E677CC7827E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="10245" windowHeight="10920" xr2:uid="{93B572C4-FF05-4AE2-8C79-3CDEABF44638}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{93B572C4-FF05-4AE2-8C79-3CDEABF44638}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="109">
   <si>
     <t>TransactionID(PK)</t>
   </si>
@@ -147,9 +147,6 @@
     <t>FTE</t>
   </si>
   <si>
-    <t>ProviderID(PK)</t>
-  </si>
-  <si>
     <t>ProviderType</t>
   </si>
   <si>
@@ -346,6 +343,15 @@
   </si>
   <si>
     <t>JOIN using Patient.PatientNbr = PatientSurvey.SurveyNbr</t>
+  </si>
+  <si>
+    <t>PhysicianID(PK)</t>
+  </si>
+  <si>
+    <t>DiagnosisCodeID(PK)</t>
+  </si>
+  <si>
+    <t>CPTCodeID(PK)</t>
   </si>
 </sst>
 </file>
@@ -736,8 +742,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1A8144B-ABD4-4E99-9252-F749DDDE434A}">
   <dimension ref="A1:J67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A51" workbookViewId="0">
-      <selection activeCell="C54" sqref="C54"/>
+    <sheetView tabSelected="1" topLeftCell="A53" workbookViewId="0">
+      <selection activeCell="B73" sqref="B73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -759,19 +765,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="B1" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="C1" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="D1" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="C1" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>55</v>
-      </c>
       <c r="E1" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -782,10 +788,10 @@
         <v>0</v>
       </c>
       <c r="C2" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>58</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>59</v>
       </c>
       <c r="E2" s="1"/>
     </row>
@@ -797,10 +803,10 @@
         <v>1</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E3" s="1"/>
     </row>
@@ -812,10 +818,10 @@
         <v>2</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E4" s="1"/>
     </row>
@@ -827,13 +833,13 @@
         <v>32</v>
       </c>
       <c r="C5" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="E5" s="1" t="s">
         <v>63</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -844,13 +850,13 @@
         <v>9</v>
       </c>
       <c r="C6" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E6" s="1" t="s">
         <v>65</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -861,13 +867,13 @@
         <v>5</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -878,13 +884,13 @@
         <v>3</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -895,10 +901,10 @@
         <v>4</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E9" s="1"/>
     </row>
@@ -910,13 +916,13 @@
         <v>6</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>6</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -927,10 +933,10 @@
         <v>10</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E11" s="1"/>
     </row>
@@ -942,10 +948,10 @@
         <v>11</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E12" s="1"/>
     </row>
@@ -957,10 +963,10 @@
         <v>12</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E13" s="6"/>
     </row>
@@ -979,10 +985,10 @@
         <v>30</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E15" s="1"/>
     </row>
@@ -991,13 +997,13 @@
         <v>7</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E16" s="1"/>
     </row>
@@ -1006,13 +1012,13 @@
         <v>7</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C17" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="D17" s="1" t="s">
         <v>73</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>74</v>
       </c>
       <c r="E17" s="1"/>
     </row>
@@ -1024,7 +1030,7 @@
         <v>13</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>13</v>
@@ -1039,7 +1045,7 @@
         <v>14</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>14</v>
@@ -1054,7 +1060,7 @@
         <v>15</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>15</v>
@@ -1069,7 +1075,7 @@
         <v>25</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>25</v>
@@ -1084,13 +1090,13 @@
         <v>26</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
@@ -1098,13 +1104,13 @@
         <v>7</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E23" s="1"/>
     </row>
@@ -1116,13 +1122,13 @@
         <v>27</v>
       </c>
       <c r="C24" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="D24" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="D24" s="1" t="s">
-        <v>78</v>
-      </c>
       <c r="E24" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
@@ -1130,16 +1136,16 @@
         <v>7</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
@@ -1147,16 +1153,16 @@
         <v>7</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
@@ -1164,16 +1170,16 @@
         <v>7</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
@@ -1184,13 +1190,13 @@
         <v>16</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D28" s="1" t="s">
         <v>16</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
@@ -1201,13 +1207,13 @@
         <v>17</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
@@ -1218,13 +1224,13 @@
         <v>18</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
@@ -1235,13 +1241,13 @@
         <v>19</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
@@ -1252,13 +1258,13 @@
         <v>20</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
@@ -1269,13 +1275,13 @@
         <v>21</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
@@ -1283,13 +1289,13 @@
         <v>7</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E34" s="1"/>
     </row>
@@ -1298,13 +1304,13 @@
         <v>7</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E35" s="1"/>
     </row>
@@ -1316,7 +1322,7 @@
         <v>22</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D36" s="1" t="s">
         <v>22</v>
@@ -1331,7 +1337,7 @@
         <v>23</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D37" s="1" t="s">
         <v>23</v>
@@ -1346,7 +1352,7 @@
         <v>29</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D38" s="1" t="s">
         <v>29</v>
@@ -1361,10 +1367,10 @@
         <v>28</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E39" s="1"/>
     </row>
@@ -1376,7 +1382,7 @@
         <v>24</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D40" s="1" t="s">
         <v>24</v>
@@ -1395,13 +1401,13 @@
         <v>35</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>40</v>
+        <v>106</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E42" s="1"/>
     </row>
@@ -1413,10 +1419,10 @@
         <v>36</v>
       </c>
       <c r="C43" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="D43" s="1" t="s">
         <v>95</v>
-      </c>
-      <c r="D43" s="1" t="s">
-        <v>96</v>
       </c>
       <c r="E43" s="1"/>
     </row>
@@ -1425,13 +1431,13 @@
         <v>35</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E44" s="1"/>
     </row>
@@ -1443,7 +1449,7 @@
         <v>13</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D45" s="1" t="s">
         <v>13</v>
@@ -1458,7 +1464,7 @@
         <v>14</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D46" s="1" t="s">
         <v>14</v>
@@ -1473,7 +1479,7 @@
         <v>15</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D47" s="1" t="s">
         <v>15</v>
@@ -1488,7 +1494,7 @@
         <v>39</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D48" s="1" t="s">
         <v>39</v>
@@ -1500,13 +1506,13 @@
         <v>35</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E49" s="6"/>
     </row>
@@ -1524,7 +1530,7 @@
         <v>38</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
@@ -1542,10 +1548,10 @@
         <v>33</v>
       </c>
       <c r="C52" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D52" s="1" t="s">
         <v>62</v>
-      </c>
-      <c r="D52" s="1" t="s">
-        <v>63</v>
       </c>
       <c r="E52" s="1"/>
     </row>
@@ -1557,10 +1563,10 @@
         <v>34</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E53" s="1"/>
     </row>
@@ -1569,13 +1575,13 @@
         <v>31</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E54" s="1"/>
     </row>
@@ -1584,13 +1590,13 @@
         <v>31</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E55" s="1"/>
     </row>
@@ -1602,7 +1608,7 @@
         <v>22</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D56" s="1" t="s">
         <v>22</v>
@@ -1617,7 +1623,7 @@
         <v>23</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D57" s="1" t="s">
         <v>23</v>
@@ -1632,10 +1638,10 @@
         <v>28</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E58" s="1"/>
     </row>
@@ -1647,7 +1653,7 @@
         <v>24</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D59" s="1" t="s">
         <v>24</v>
@@ -1663,98 +1669,97 @@
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>42</v>
+        <v>107</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E61" s="6"/>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B62" s="2" t="s">
         <v>43</v>
       </c>
       <c r="C62" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="D62" s="1" t="s">
         <v>101</v>
-      </c>
-      <c r="D62" s="1" t="s">
-        <v>102</v>
       </c>
       <c r="E62" s="6"/>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E63" s="6"/>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" s="1"/>
-      <c r="B64" s="1"/>
       <c r="C64" s="1"/>
       <c r="D64" s="1"/>
       <c r="E64" s="1"/>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>48</v>
+        <v>108</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E65" s="1"/>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B66" s="2" t="s">
         <v>49</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E66" s="1"/>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C67" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="D67" s="1" t="s">
         <v>104</v>
-      </c>
-      <c r="D67" s="1" t="s">
-        <v>105</v>
       </c>
       <c r="E67" s="1"/>
     </row>

</xml_diff>